<commit_message>
Added homework tasks distribution list
</commit_message>
<xml_diff>
--- a/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
+++ b/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Development\.NET\Practical-Software-Development-11D\src\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C3FF43-1E09-46B7-8308-208CA76BD3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839669AF-B0B2-4667-BC5A-5B88A9410086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9815A92-6A38-4E98-B8C2-F5AC02CF0389}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,8 +506,12 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -516,8 +520,12 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -526,8 +534,12 @@
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -546,8 +558,12 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -556,8 +572,12 @@
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -566,8 +586,12 @@
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -576,8 +600,12 @@
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -586,8 +614,12 @@
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -596,8 +628,12 @@
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -606,8 +642,12 @@
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -616,8 +656,12 @@
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -626,8 +670,12 @@
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D14">

</xml_diff>

<commit_message>
Modified the homework distribution list
</commit_message>
<xml_diff>
--- a/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
+++ b/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Development\.NET\Practical-Software-Development-11D\src\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839669AF-B0B2-4667-BC5A-5B88A9410086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0705CBC-7771-4D55-8D09-E3D6BFF64558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9815A92-6A38-4E98-B8C2-F5AC02CF0389}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,8 +548,12 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">

</xml_diff>

<commit_message>
Updated the homework tasks distribution sheet
</commit_message>
<xml_diff>
--- a/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
+++ b/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Development\.NET\Practical-Software-Development-11D\src\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0705CBC-7771-4D55-8D09-E3D6BFF64558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AA4DB0-2434-4D2E-9374-569239C08227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9815A92-6A38-4E98-B8C2-F5AC02CF0389}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>№ в клас</t>
   </si>
@@ -76,6 +76,39 @@
   </si>
   <si>
     <t>Християн Г. Русев</t>
+  </si>
+  <si>
+    <t>№ Задача - Преработка и постепенни промени</t>
+  </si>
+  <si>
+    <t>Задачи от темата: Преработка и постепенни промени</t>
+  </si>
+  <si>
+    <t>1. OrdersBadCode</t>
+  </si>
+  <si>
+    <t>2. RotatingWalkInMatrixBadCode</t>
+  </si>
+  <si>
+    <t>3. UnknownMethodBadCode</t>
+  </si>
+  <si>
+    <t>4. HighQualityMethodsBadCode</t>
+  </si>
+  <si>
+    <t>5. YoloSnakeBadCode</t>
+  </si>
+  <si>
+    <t>6. FiveSpecialLettersBadCode</t>
+  </si>
+  <si>
+    <t>Задача по желание MinesweeperBadCode</t>
+  </si>
+  <si>
+    <t>Да се документират всички задачи (техните методи и класове) чрез вградените средства на Visual Studio за XML документация</t>
+  </si>
+  <si>
+    <t>Вижте презентацията за документиране и коментиране на кода</t>
   </si>
 </sst>
 </file>
@@ -468,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CE112C-BB1D-4220-B703-297D8F46EDE4}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +512,7 @@
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
     <col min="3" max="3" width="56.44140625" customWidth="1"/>
     <col min="4" max="4" width="67.44140625" customWidth="1"/>
-    <col min="5" max="5" width="33.88671875" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" customWidth="1"/>
     <col min="6" max="6" width="41.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -496,7 +529,9 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -681,9 +716,59 @@
         <v>3</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D14">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -695,7 +780,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D14">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -706,6 +791,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E1">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the winter holiday homework distribution sheet
</commit_message>
<xml_diff>
--- a/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
+++ b/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Development\.NET\Practical-Software-Development-11D\src\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AA4DB0-2434-4D2E-9374-569239C08227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981BE6EA-F341-4ADD-BAB3-83FC19F552D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9815A92-6A38-4E98-B8C2-F5AC02CF0389}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>№ Задача - Преработка и постепенни промени</t>
   </si>
   <si>
-    <t>Задачи от темата: Преработка и постепенни промени</t>
-  </si>
-  <si>
     <t>1. OrdersBadCode</t>
   </si>
   <si>
@@ -105,10 +102,13 @@
     <t>Задача по желание MinesweeperBadCode</t>
   </si>
   <si>
-    <t>Да се документират всички задачи (техните методи и класове) чрез вградените средства на Visual Studio за XML документация</t>
-  </si>
-  <si>
     <t>Вижте презентацията за документиране и коментиране на кода</t>
+  </si>
+  <si>
+    <t>4 задача. Да се документират всички задачи (техните методи и класове) чрез вградените средства на Visual Studio за XML документация</t>
+  </si>
+  <si>
+    <t>Задачи от темата: Преработка и постепенни промени, може да намерите задачите на: https://github.com/plamenna-petrova/Practical-Software-Development-11D/tree/master/src/Exercises/Refactoring-And-Progressive-Changes и условията: https://github.com/plamenna-petrova/Practical-Software-Development-11D/tree/master/src/Files/4.%20%D0%9F%D1%80%D0%B5%D1%80%D0%B0%D0%B1%D0%BE%D1%82%D0%BA%D0%B0%20%D0%B8%20%D0%BF%D0%BE%D1%81%D1%82%D0%B5%D0%BF%D0%B5%D0%BD%D0%BD%D0%B8%20%D0%BF%D1%80%D0%BE%D0%BC%D0%B5%D0%BD%D0%B8</t>
   </si>
 </sst>
 </file>
@@ -147,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,11 +170,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -182,6 +193,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CE112C-BB1D-4220-B703-297D8F46EDE4}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,6 +559,9 @@
       <c r="D2" s="1">
         <v>5</v>
       </c>
+      <c r="E2" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -561,6 +576,9 @@
       <c r="D3" s="1">
         <v>5</v>
       </c>
+      <c r="E3" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -575,6 +593,9 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
+      <c r="E4" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -589,6 +610,9 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -603,6 +627,9 @@
       <c r="D6" s="1">
         <v>2</v>
       </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -617,6 +644,9 @@
       <c r="D7" s="1">
         <v>6</v>
       </c>
+      <c r="E7" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -631,6 +661,9 @@
       <c r="D8" s="1">
         <v>2</v>
       </c>
+      <c r="E8" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -645,6 +678,9 @@
       <c r="D9" s="1">
         <v>4</v>
       </c>
+      <c r="E9" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -659,6 +695,9 @@
       <c r="D10" s="1">
         <v>6</v>
       </c>
+      <c r="E10" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -673,6 +712,9 @@
       <c r="D11" s="1">
         <v>7</v>
       </c>
+      <c r="E11" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -687,6 +729,9 @@
       <c r="D12" s="1">
         <v>4</v>
       </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -701,6 +746,9 @@
       <c r="D13" s="1">
         <v>7</v>
       </c>
+      <c r="E13" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -715,45 +763,48 @@
       <c r="D14" s="1">
         <v>3</v>
       </c>
+      <c r="E14" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
@@ -763,11 +814,11 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D14">
+  <conditionalFormatting sqref="A1:D14 E2:E14">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -779,7 +830,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:D14">
+  <conditionalFormatting sqref="A2:E14">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added Homework distribution file for the first homework of the second term
</commit_message>
<xml_diff>
--- a/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
+++ b/src/Homeworks/Разпределение на задачите за първата домашна работа за първия срок.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Development\.NET\Practical-Software-Development-11D\src\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981BE6EA-F341-4ADD-BAB3-83FC19F552D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02721AD-D241-40A4-9B7F-5CC90D492C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9815A92-6A38-4E98-B8C2-F5AC02CF0389}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CE112C-BB1D-4220-B703-297D8F46EDE4}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>